<commit_message>
updating a couple of missing values
</commit_message>
<xml_diff>
--- a/sagehen_3lay_modsim/Ocsillations_2.xlsx
+++ b/sagehen_3lay_modsim/Ocsillations_2.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22998" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22998" windowHeight="8340" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="spatial_org (1-based iseg vals)" sheetId="2" r:id="rId2"/>
     <sheet name="9-17-1988_Conv_Issues" sheetId="3" r:id="rId3"/>
     <sheet name="9-17-1988_Conv_Issues_LAK_Vol" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="67">
   <si>
     <t>EXCHANGE</t>
   </si>
@@ -332,15 +333,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -358,16 +359,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3728,10 +3719,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:R53">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>-1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4417,18 +4408,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
@@ -8865,10 +8856,10 @@
     <mergeCell ref="B1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="O4:Y55">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>-1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8881,31 +8872,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="25.68359375" customWidth="1"/>
     <col min="2" max="11" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.20703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="3.20703125" style="6" customWidth="1"/>
     <col min="13" max="13" width="12.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
@@ -9036,39 +9027,39 @@
         <v>245.211502075195</v>
       </c>
       <c r="M4" s="1">
-        <f>B4-C4</f>
+        <f t="shared" ref="M4:U4" si="0">B4-C4</f>
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f>C4-D4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <f>D4-E4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <f>E4-F4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <f>F4-G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <f>G4-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S4" s="1">
-        <f>H4-I4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T4" s="1">
-        <f>I4-J4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <f>J4-K4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9107,39 +9098,39 @@
         <v>56.372688293457003</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" ref="M5:M58" si="0">B5-C5</f>
+        <f t="shared" ref="M5:M58" si="1">B5-C5</f>
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <f>C5-D5</f>
+        <f t="shared" ref="N5:N19" si="2">C5-D5</f>
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <f>D5-E5</f>
+        <f t="shared" ref="O5:O19" si="3">D5-E5</f>
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <f>E5-F5</f>
+        <f t="shared" ref="P5:P19" si="4">E5-F5</f>
         <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <f>F5-G5</f>
+        <f t="shared" ref="Q5:Q19" si="5">F5-G5</f>
         <v>0</v>
       </c>
       <c r="R5" s="1">
-        <f>G5-H5</f>
+        <f t="shared" ref="R5:R19" si="6">G5-H5</f>
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <f>H5-I5</f>
+        <f t="shared" ref="S5:S19" si="7">H5-I5</f>
         <v>0</v>
       </c>
       <c r="T5" s="1">
-        <f>I5-J5</f>
+        <f t="shared" ref="T5:T19" si="8">I5-J5</f>
         <v>0</v>
       </c>
       <c r="U5" s="1">
-        <f>J5-K5</f>
+        <f t="shared" ref="U5:U19" si="9">J5-K5</f>
         <v>0</v>
       </c>
     </row>
@@ -9178,39 +9169,39 @@
         <v>-60.450332641601499</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.826660156200262E-3</v>
       </c>
       <c r="N6" s="1">
-        <f>C6-D6</f>
+        <f t="shared" si="2"/>
         <v>2.3193359375E-3</v>
       </c>
       <c r="O6" s="1">
-        <f>D6-E6</f>
+        <f t="shared" si="3"/>
         <v>-1.5045166015603684E-2</v>
       </c>
       <c r="P6" s="1">
-        <f>E6-F6</f>
+        <f t="shared" si="4"/>
         <v>-1.7196655273401973E-2</v>
       </c>
       <c r="Q6" s="1">
-        <f>F6-G6</f>
+        <f t="shared" si="5"/>
         <v>-4.0283203125E-3</v>
       </c>
       <c r="R6" s="1">
-        <f>G6-H6</f>
+        <f t="shared" si="6"/>
         <v>-7.6293945298289145E-5</v>
       </c>
       <c r="S6" s="1">
-        <f>H6-I6</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T6" s="1">
-        <f>I6-J6</f>
+        <f t="shared" si="8"/>
         <v>-4.5776367201710855E-5</v>
       </c>
       <c r="U6" s="1">
-        <f>J6-K6</f>
+        <f t="shared" si="9"/>
         <v>-1.5258789098027137E-5</v>
       </c>
     </row>
@@ -9249,39 +9240,39 @@
         <v>383.55389404296801</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5258789096606051E-4</v>
       </c>
       <c r="N7" s="1">
-        <f>C7-D7</f>
+        <f t="shared" si="2"/>
         <v>3.0517578011313162E-5</v>
       </c>
       <c r="O7" s="1">
-        <f>D7-E7</f>
+        <f t="shared" si="3"/>
         <v>-3.9154052735000278E-2</v>
       </c>
       <c r="P7" s="1">
-        <f>E7-F7</f>
+        <f t="shared" si="4"/>
         <v>1.8615722660229039E-3</v>
       </c>
       <c r="Q7" s="1">
-        <f>F7-G7</f>
+        <f t="shared" si="5"/>
         <v>3.0517578096578291E-4</v>
       </c>
       <c r="R7" s="1">
-        <f>G7-H7</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S7" s="1">
-        <f>H7-I7</f>
+        <f t="shared" si="7"/>
         <v>-1.2207031198840923E-4</v>
       </c>
       <c r="T7" s="1">
-        <f>I7-J7</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U7" s="1">
-        <f>J7-K7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9320,39 +9311,39 @@
         <v>6.6650390625E-2</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f>C8-D8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <f>D8-E8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <f>E8-F8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <f>F8-G8</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R8" s="1">
-        <f>G8-H8</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S8" s="1">
-        <f>H8-I8</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <f>I8-J8</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U8" s="1">
-        <f>J8-K8</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9391,39 +9382,39 @@
         <v>918.69140625</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.953125E-3</v>
       </c>
       <c r="N9" s="1">
-        <f>C9-D9</f>
+        <f t="shared" si="2"/>
         <v>1.953125E-3</v>
       </c>
       <c r="O9" s="1">
-        <f>D9-E9</f>
+        <f t="shared" si="3"/>
         <v>6.8359375E-2</v>
       </c>
       <c r="P9" s="1">
-        <f>E9-F9</f>
+        <f t="shared" si="4"/>
         <v>6.4453125E-2</v>
       </c>
       <c r="Q9" s="1">
-        <f>F9-G9</f>
+        <f t="shared" si="5"/>
         <v>1.171875E-2</v>
       </c>
       <c r="R9" s="1">
-        <f>G9-H9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S9" s="1">
-        <f>H9-I9</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T9" s="1">
-        <f>I9-J9</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U9" s="1">
-        <f>J9-K9</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9462,39 +9453,39 @@
         <v>163.20062255859301</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f>C10-D10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <f>D10-E10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <f>E10-F10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <f>F10-G10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R10" s="1">
-        <f>G10-H10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S10" s="1">
-        <f>H10-I10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T10" s="1">
-        <f>I10-J10</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U10" s="1">
-        <f>J10-K10</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9533,39 +9524,39 @@
         <v>68.386863708496094</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f>C11-D11</f>
+        <f t="shared" si="2"/>
         <v>7.6293946023042736E-6</v>
       </c>
       <c r="O11" s="1">
-        <f>D11-E11</f>
+        <f t="shared" si="3"/>
         <v>-3.7368774414090922E-2</v>
       </c>
       <c r="P11" s="1">
-        <f>E11-F11</f>
+        <f t="shared" si="4"/>
         <v>1.3122558593892109E-3</v>
       </c>
       <c r="Q11" s="1">
-        <f>F11-G11</f>
+        <f t="shared" si="5"/>
         <v>9.918212890625E-5</v>
       </c>
       <c r="R11" s="1">
-        <f>G11-H11</f>
+        <f t="shared" si="6"/>
         <v>-6.8664550795460855E-5</v>
       </c>
       <c r="S11" s="1">
-        <f>H11-I11</f>
+        <f t="shared" si="7"/>
         <v>-4.5776367201710855E-5</v>
       </c>
       <c r="T11" s="1">
-        <f>I11-J11</f>
+        <f t="shared" si="8"/>
         <v>7.6293945028282906E-6</v>
       </c>
       <c r="U11" s="1">
-        <f>J11-K11</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9604,39 +9595,39 @@
         <v>633.57855224609295</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f>C12-D12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <f>D12-E12</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
-        <f>E12-F12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <f>F12-G12</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
-        <f>G12-H12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <f>H12-I12</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="1">
-        <f>I12-J12</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U12" s="1">
-        <f>J12-K12</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9675,39 +9666,39 @@
         <v>2008.63159179687</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <f>C13-D13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13" s="1">
-        <f>D13-E13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13" s="1">
-        <f>E13-F13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <f>F13-G13</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R13" s="1">
-        <f>G13-H13</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S13" s="1">
-        <f>H13-I13</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <f>I13-J13</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U13" s="1">
-        <f>J13-K13</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9746,39 +9737,39 @@
         <v>583.13671875</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.765625E-3</v>
       </c>
       <c r="N14" s="1">
-        <f>C14-D14</f>
+        <f t="shared" si="2"/>
         <v>1.953125E-3</v>
       </c>
       <c r="O14" s="1">
-        <f>D14-E14</f>
+        <f t="shared" si="3"/>
         <v>6.8359375E-2</v>
       </c>
       <c r="P14" s="1">
-        <f>E14-F14</f>
+        <f t="shared" si="4"/>
         <v>2.5390625E-2</v>
       </c>
       <c r="Q14" s="1">
-        <f>F14-G14</f>
+        <f t="shared" si="5"/>
         <v>9.765625E-3</v>
       </c>
       <c r="R14" s="1">
-        <f>G14-H14</f>
+        <f t="shared" si="6"/>
         <v>1.953125E-3</v>
       </c>
       <c r="S14" s="1">
-        <f>H14-I14</f>
+        <f t="shared" si="7"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="T14" s="1">
-        <f>I14-J14</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U14" s="1">
-        <f>J14-K14</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9817,39 +9808,39 @@
         <v>52.073196411132798</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <f>C15-D15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f>D15-E15</f>
+        <f t="shared" si="3"/>
         <v>-3.8146973011521368E-6</v>
       </c>
       <c r="P15" s="1">
-        <f>E15-F15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <f>F15-G15</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R15" s="1">
-        <f>G15-H15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S15" s="1">
-        <f>H15-I15</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T15" s="1">
-        <f>I15-J15</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U15" s="1">
-        <f>J15-K15</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9888,39 +9879,39 @@
         <v>-52.412109375</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.568359375</v>
       </c>
       <c r="N16" s="1">
-        <f>C16-D16</f>
+        <f t="shared" si="2"/>
         <v>0.1328125</v>
       </c>
       <c r="O16" s="1">
-        <f>D16-E16</f>
+        <f t="shared" si="3"/>
         <v>1.916015625</v>
       </c>
       <c r="P16" s="1">
-        <f>E16-F16</f>
+        <f t="shared" si="4"/>
         <v>-1.05859375</v>
       </c>
       <c r="Q16" s="1">
-        <f>F16-G16</f>
+        <f t="shared" si="5"/>
         <v>3.515625E-2</v>
       </c>
       <c r="R16" s="1">
-        <f>G16-H16</f>
+        <f t="shared" si="6"/>
         <v>3.3203125E-2</v>
       </c>
       <c r="S16" s="1">
-        <f>H16-I16</f>
+        <f t="shared" si="7"/>
         <v>-2.1484375E-2</v>
       </c>
       <c r="T16" s="1">
-        <f>I16-J16</f>
+        <f t="shared" si="8"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="U16" s="1">
-        <f>J16-K16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9959,39 +9950,39 @@
         <v>229.06405639648401</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8615722659944822E-3</v>
       </c>
       <c r="N17" s="1">
-        <f>C17-D17</f>
+        <f t="shared" si="2"/>
         <v>3.6621093698840923E-4</v>
       </c>
       <c r="O17" s="1">
-        <f>D17-E17</f>
+        <f t="shared" si="3"/>
         <v>-7.4615478514999722E-2</v>
       </c>
       <c r="P17" s="1">
-        <f>E17-F17</f>
+        <f t="shared" si="4"/>
         <v>-1.4343261719886868E-3</v>
       </c>
       <c r="Q17" s="1">
-        <f>F17-G17</f>
+        <f t="shared" si="5"/>
         <v>4.7302246099434342E-4</v>
       </c>
       <c r="R17" s="1">
-        <f>G17-H17</f>
+        <f t="shared" si="6"/>
         <v>3.0517578011313162E-5</v>
       </c>
       <c r="S17" s="1">
-        <f>H17-I17</f>
+        <f t="shared" si="7"/>
         <v>-2.1362304701710855E-4</v>
       </c>
       <c r="T17" s="1">
-        <f>I17-J17</f>
+        <f t="shared" si="8"/>
         <v>1.5258789005656581E-5</v>
       </c>
       <c r="U17" s="1">
-        <f>J17-K17</f>
+        <f t="shared" si="9"/>
         <v>-1.5258789005656581E-5</v>
       </c>
     </row>
@@ -10030,39 +10021,39 @@
         <v>6.912109375</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.90625E-3</v>
       </c>
       <c r="N18" s="1">
-        <f>C18-D18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O18" s="1">
-        <f>D18-E18</f>
+        <f t="shared" si="3"/>
         <v>1.7578125E-2</v>
       </c>
       <c r="P18" s="1">
-        <f>E18-F18</f>
+        <f t="shared" si="4"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="Q18" s="1">
-        <f>F18-G18</f>
+        <f t="shared" si="5"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="R18" s="1">
-        <f>G18-H18</f>
+        <f t="shared" si="6"/>
         <v>1.953125E-3</v>
       </c>
       <c r="S18" s="1">
-        <f>H18-I18</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T18" s="1">
-        <f>I18-J18</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U18" s="1">
-        <f>J18-K18</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -10101,39 +10092,39 @@
         <v>44.5546875</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.83203125E-2</v>
       </c>
       <c r="N19" s="1">
-        <f>C19-D19</f>
+        <f t="shared" si="2"/>
         <v>1.07421875E-2</v>
       </c>
       <c r="O19" s="1">
-        <f>D19-E19</f>
+        <f t="shared" si="3"/>
         <v>4.19921875E-2</v>
       </c>
       <c r="P19" s="1">
-        <f>E19-F19</f>
+        <f t="shared" si="4"/>
         <v>2.63671875E-2</v>
       </c>
       <c r="Q19" s="1">
-        <f>F19-G19</f>
+        <f t="shared" si="5"/>
         <v>-9.765625E-4</v>
       </c>
       <c r="R19" s="1">
-        <f>G19-H19</f>
+        <f t="shared" si="6"/>
         <v>-3.90625E-3</v>
       </c>
       <c r="S19" s="1">
-        <f>H19-I19</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
-        <f>I19-J19</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U19" s="1">
-        <f>J19-K19</f>
+        <f t="shared" si="9"/>
         <v>9.765625E-4</v>
       </c>
     </row>
@@ -10172,39 +10163,39 @@
         <v>247.31362915039</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" ref="N20:N58" si="1">C20-D20</f>
+        <f t="shared" ref="M20:N58" si="10">C20-D20</f>
         <v>-2.44140625E-3</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" ref="O20:O58" si="2">D20-E20</f>
+        <f t="shared" ref="O20:O58" si="11">D20-E20</f>
         <v>1.8310546900579538E-4</v>
       </c>
       <c r="P20" s="1">
-        <f t="shared" ref="P20:P58" si="3">E20-F20</f>
+        <f t="shared" ref="P20:P58" si="12">E20-F20</f>
         <v>1.5258789005656581E-5</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" ref="Q20:Q58" si="4">F20-G20</f>
+        <f t="shared" ref="Q20:Q58" si="13">F20-G20</f>
         <v>1.2207031198840923E-4</v>
       </c>
       <c r="R20" s="1">
-        <f t="shared" ref="R20:R58" si="5">G20-H20</f>
+        <f t="shared" ref="R20:R58" si="14">G20-H20</f>
         <v>-6.1035155994204615E-5</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" ref="S20:S58" si="6">H20-I20</f>
+        <f t="shared" ref="S20:S58" si="15">H20-I20</f>
         <v>0</v>
       </c>
       <c r="T20" s="1">
-        <f t="shared" ref="T20:T58" si="7">I20-J20</f>
+        <f t="shared" ref="T20:T58" si="16">I20-J20</f>
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <f t="shared" ref="U20:U58" si="8">J20-K20</f>
+        <f t="shared" ref="U20:U58" si="17">J20-K20</f>
         <v>0</v>
       </c>
     </row>
@@ -10243,39 +10234,39 @@
         <v>182.466796875</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.3046875</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-0.216796875</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>1.953125E-3</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.953125E-3</v>
       </c>
       <c r="R21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="S21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10314,39 +10305,39 @@
         <v>711.97613525390602</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3984375E-2</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>-1.4031982421880684</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.83087158203102263</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-1.3793945312045253E-2</v>
       </c>
       <c r="Q22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>5.2276611328011313E-2</v>
       </c>
       <c r="R22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>-8.3068847656022626E-2</v>
       </c>
       <c r="S22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.4373779297102374E-2</v>
       </c>
       <c r="T22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>-7.32421875E-4</v>
       </c>
       <c r="U22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.3427734369315658E-3</v>
       </c>
     </row>
@@ -10385,39 +10376,39 @@
         <v>0</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10456,39 +10447,39 @@
         <v>503.46484375</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4921875E-2</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>7.8125E-3</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.17578125</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-0.10546875</v>
       </c>
       <c r="Q24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-5.859375E-3</v>
       </c>
       <c r="R24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1.953125E-3</v>
       </c>
       <c r="S24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="T24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10527,39 +10518,39 @@
         <v>-217.7685546875</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8125E-3</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>-2.9296875E-3</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>9.765625E-4</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="Q25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-1.953125E-3</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10598,39 +10589,39 @@
         <v>811.44140625</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.294921875</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>8.3984375E-2</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.7421875</v>
       </c>
       <c r="P26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-0.251953125</v>
       </c>
       <c r="Q26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-0.2177734375</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>-1.5625E-2</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>4.8828125E-3</v>
       </c>
       <c r="T26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>9.765625E-4</v>
       </c>
       <c r="U26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10713,39 +10704,39 @@
         <v>1407.0559464990999</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.13671875</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.11328125</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-1.171875E-2</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>3.90625E-3</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10784,39 +10775,39 @@
         <v>-300.28532016277302</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>-0.24755859375</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-5.0170898438011591E-2</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0.14997863769599462</v>
       </c>
       <c r="Q29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-5.0109863281988964E-2</v>
       </c>
       <c r="R29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0.10006713867198869</v>
       </c>
       <c r="S29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>-0.15002441406198841</v>
       </c>
       <c r="T29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10855,39 +10846,39 @@
         <v>127007.234375</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.4453125</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.3125</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-0.2109375</v>
       </c>
       <c r="P30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0.1015625</v>
       </c>
       <c r="Q30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10926,39 +10917,39 @@
         <v>3518573.25</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-56.25</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.75</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-0.75</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>3.25</v>
       </c>
       <c r="Q31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-1.25</v>
       </c>
       <c r="R31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>-0.25</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11041,39 +11032,39 @@
         <v>0</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11112,39 +11103,39 @@
         <v>0</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11183,39 +11174,39 @@
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T35" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11254,39 +11245,39 @@
         <v>0</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11325,39 +11316,39 @@
         <v>0</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S37" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11396,39 +11387,39 @@
         <v>0</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S38" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11467,39 +11458,39 @@
         <v>0</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q39" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U39" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11538,39 +11529,39 @@
         <v>0</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q40" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S40" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11609,39 +11600,39 @@
         <v>0</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q41" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S41" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11680,39 +11671,39 @@
         <v>0</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q42" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11751,39 +11742,39 @@
         <v>0</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q43" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R43" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S43" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11822,39 +11813,39 @@
         <v>0</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q44" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R44" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S44" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11893,39 +11884,39 @@
         <v>0</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q45" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -11964,39 +11955,39 @@
         <v>0</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q46" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S46" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12035,39 +12026,39 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12106,39 +12097,39 @@
         <v>0</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q48" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S48" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12177,39 +12168,39 @@
         <v>0</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q49" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S49" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12248,39 +12239,39 @@
         <v>19256.2</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-35.799999999999272</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>-0.2000000000007276</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.2000000000007276</v>
       </c>
       <c r="P50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-0.10000000000218279</v>
       </c>
       <c r="Q50" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12319,39 +12310,39 @@
         <v>373.7</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
       <c r="N51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.69999999999998863</v>
       </c>
       <c r="P51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>-3.0999999999989996</v>
       </c>
       <c r="Q51" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.1999999999990223</v>
       </c>
       <c r="R51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>9.9999999999965894E-2</v>
       </c>
       <c r="S51" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.10000000000002274</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12390,39 +12381,39 @@
         <v>0</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q52" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S52" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12461,39 +12452,39 @@
         <v>0</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q53" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R53" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S53" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12532,39 +12523,39 @@
         <v>12217.8</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.9999999998544808E-2</v>
       </c>
       <c r="N54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q54" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12603,39 +12594,39 @@
         <v>0</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12643,6 +12634,9 @@
       <c r="A56" t="s">
         <v>65</v>
       </c>
+      <c r="B56" s="1">
+        <v>1270000</v>
+      </c>
       <c r="C56" s="1">
         <v>1270000</v>
       </c>
@@ -12670,37 +12664,40 @@
       <c r="K56" s="1">
         <v>1270000</v>
       </c>
-      <c r="M56" s="1"/>
+      <c r="M56" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="N56" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q56" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S56" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12708,6 +12705,9 @@
       <c r="A57" t="s">
         <v>66</v>
       </c>
+      <c r="B57" s="1">
+        <v>35179398</v>
+      </c>
       <c r="C57" s="1">
         <v>35185753</v>
       </c>
@@ -12735,82 +12735,84 @@
       <c r="K57" s="1">
         <v>35185733</v>
       </c>
-      <c r="M57" s="1"/>
+      <c r="M57" s="1">
+        <f t="shared" si="10"/>
+        <v>-6355</v>
+      </c>
       <c r="N57" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-9</v>
       </c>
       <c r="P57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="Q57" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>-10</v>
       </c>
       <c r="R57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>-2</v>
       </c>
       <c r="S57" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>-1</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="M58" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N58" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R58" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -12823,14 +12825,120 @@
     <mergeCell ref="B1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="M4:U58">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>-1</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1015625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="1">
+        <v>127042.8828125</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1">
+        <v>127007.4375</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1">
+        <v>127007.125</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="1">
+        <v>127007.3359375</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="1">
+        <v>127007.234375</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1270000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>